<commit_message>
possibly because of my lazy prompting
</commit_message>
<xml_diff>
--- a/flashcards_template.xlsx
+++ b/flashcards_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.marks\x\flashcards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F760736A-9E00-41B6-BB9B-653DE08BB904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B8BB55-D13B-4EC5-8299-5AE18480088F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="16548" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="18780" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -355,9 +355,6 @@
     <t>img/3.jpg</t>
   </si>
   <si>
-    <t>img/4.jpg</t>
-  </si>
-  <si>
     <t>img/5.jpg</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
     <t>img/17.jpg</t>
   </si>
   <si>
-    <t>img/7.jpg</t>
-  </si>
-  <si>
     <t>Internal Controls</t>
   </si>
   <si>
@@ -751,10 +745,16 @@
     <t>nature, timing</t>
   </si>
   <si>
-    <t>img/15.jpg</t>
-  </si>
-  <si>
     <t>img/16.jpg</t>
+  </si>
+  <si>
+    <t>img/4.png</t>
+  </si>
+  <si>
+    <t>img/7.jpeg</t>
+  </si>
+  <si>
+    <t>img/15.png</t>
   </si>
 </sst>
 </file>
@@ -1124,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C56" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1502,7 +1502,7 @@
         <v>91</v>
       </c>
       <c r="G16" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1525,7 +1525,7 @@
         <v>92</v>
       </c>
       <c r="G17" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1548,7 +1548,7 @@
         <v>94</v>
       </c>
       <c r="G18" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1571,7 +1571,7 @@
         <v>95</v>
       </c>
       <c r="G19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1594,7 +1594,7 @@
         <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1617,7 +1617,7 @@
         <v>96</v>
       </c>
       <c r="G21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1640,7 +1640,7 @@
         <v>88</v>
       </c>
       <c r="G22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1663,7 +1663,7 @@
         <v>97</v>
       </c>
       <c r="G23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1686,7 +1686,7 @@
         <v>98</v>
       </c>
       <c r="G24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1709,7 +1709,7 @@
         <v>77</v>
       </c>
       <c r="G25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1732,7 +1732,7 @@
         <v>78</v>
       </c>
       <c r="G26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1755,7 +1755,7 @@
         <v>99</v>
       </c>
       <c r="G27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1778,7 +1778,7 @@
         <v>80</v>
       </c>
       <c r="G28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1801,7 +1801,7 @@
         <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1824,7 +1824,7 @@
         <v>101</v>
       </c>
       <c r="G30" t="s">
-        <v>115</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1847,7 +1847,7 @@
         <v>102</v>
       </c>
       <c r="G31" t="s">
-        <v>115</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1870,7 +1870,7 @@
         <v>103</v>
       </c>
       <c r="G32" t="s">
-        <v>115</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1893,7 +1893,7 @@
         <v>104</v>
       </c>
       <c r="G33" t="s">
-        <v>115</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1916,7 +1916,7 @@
         <v>105</v>
       </c>
       <c r="G34" t="s">
-        <v>115</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1939,996 +1939,996 @@
         <v>106</v>
       </c>
       <c r="G35" t="s">
-        <v>115</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
         <v>116</v>
       </c>
-      <c r="B36" t="s">
-        <v>118</v>
-      </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F36" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G36" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="s">
         <v>116</v>
       </c>
-      <c r="B37" t="s">
-        <v>118</v>
-      </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G37" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" t="s">
         <v>116</v>
       </c>
-      <c r="B38" t="s">
-        <v>118</v>
-      </c>
       <c r="C38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
         <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G38" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" t="s">
         <v>116</v>
       </c>
-      <c r="B39" t="s">
-        <v>118</v>
-      </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G39" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" t="s">
         <v>116</v>
       </c>
-      <c r="B40" t="s">
-        <v>118</v>
-      </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
       </c>
       <c r="E40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F40" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G40" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F41" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D42" t="s">
         <v>76</v>
       </c>
       <c r="E42" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F42" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F43" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G43" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
       </c>
       <c r="E44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F44" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G44" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B45" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C45" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F45" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G45" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D46" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E46" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F46" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G46" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
       </c>
       <c r="E47" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F47" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
         <v>76</v>
       </c>
       <c r="E48" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F48" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G48" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C49" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E49" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F49" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G49" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F50" t="s">
         <v>96</v>
       </c>
       <c r="G50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C51" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D51" t="s">
         <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F51" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G51" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B52" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D52" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E52" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F52" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G52" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B53" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C53" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F53" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G53" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C54" t="s">
+        <v>207</v>
+      </c>
+      <c r="D54" t="s">
+        <v>208</v>
+      </c>
+      <c r="E54" t="s">
+        <v>166</v>
+      </c>
+      <c r="F54" t="s">
         <v>209</v>
       </c>
-      <c r="D54" t="s">
-        <v>210</v>
-      </c>
-      <c r="E54" t="s">
-        <v>168</v>
-      </c>
-      <c r="F54" t="s">
-        <v>211</v>
-      </c>
       <c r="G54" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B55" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C55" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D55" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E55" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F55" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G55" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C56" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
       </c>
       <c r="E56" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F56" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G56" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B57" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C57" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E57" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F57" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G57" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C58" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E58" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F58" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G58" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B59" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C59" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F59" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G59" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C60" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D60" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E60" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F60" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G60" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C61" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
       </c>
       <c r="E61" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F61" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G61" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C62" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D62" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E62" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F62" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G62" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
       </c>
       <c r="E63" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F63" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G63" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D64" t="s">
         <v>16</v>
       </c>
       <c r="E64" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F64" t="s">
+        <v>227</v>
+      </c>
+      <c r="G64" t="s">
         <v>229</v>
-      </c>
-      <c r="G64" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D65" t="s">
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F65" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G65" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C66" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D66" t="s">
         <v>13</v>
       </c>
       <c r="E66" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F66" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G66" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C67" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D67" t="s">
         <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F67" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G67" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C68" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F68" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G68" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B69" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C69" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F69" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G69" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B70" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C70" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D70" t="s">
         <v>14</v>
       </c>
       <c r="E70" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F70" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G70" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D71" t="s">
         <v>76</v>
       </c>
       <c r="E71" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F71" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G71" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C72" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D72" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E72" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F72" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G72" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B73" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C73" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
       </c>
       <c r="E73" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F73" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G73" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C74" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D74" t="s">
         <v>15</v>
       </c>
       <c r="E74" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F74" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G74" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C75" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D75" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E75" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F75" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G75" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B76" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C76" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D76" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E76" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F76" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G76" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C77" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D77" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E77" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F77" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C78" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D78" t="s">
         <v>13</v>
       </c>
       <c r="E78" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F78" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>